<commit_message>
adding code to make optimal pairs
</commit_message>
<xml_diff>
--- a/data/SCIJ_MOCK_HEADERS.xlsx
+++ b/data/SCIJ_MOCK_HEADERS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harid\Documents\Spring 2022\SCIJPartnerMatching\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D9BF1F-B5C9-47D1-9D2D-06D2A05FDEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46420BA0-BB39-438A-BDBF-5F0956862D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14790" yWindow="4395" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -384,7 +384,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>